<commit_message>
Upload some additional example data files
</commit_message>
<xml_diff>
--- a/LMG 1401 Tecan F200 Log - MUF and AMC Enzyme Assays.xlsx
+++ b/LMG 1401 Tecan F200 Log - MUF and AMC Enzyme Assays.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="57">
   <si>
     <t>MUF and AMC-labeled enzyme substrates</t>
   </si>
@@ -145,9 +145,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Tecan F200 Plate Reader Sample Log, LMG 14-01, 2013-2014</t>
-  </si>
-  <si>
     <t>CTD no.</t>
   </si>
   <si>
@@ -191,6 +188,9 @@
   </si>
   <si>
     <t>J. Collins, james.r.collins@aya.yale.edu</t>
+  </si>
+  <si>
+    <t>Tecan F200 Plate Reader Sample Log, LMG 14-01, 2013-2014; this copy released as a template for Exoenzyme_plate_data_read_Tecan_F200.m</t>
   </si>
 </sst>
 </file>
@@ -778,7 +778,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -803,7 +803,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="22" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="22" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1499,10 +1498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S66"/>
+  <dimension ref="A1:S31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1531,7 +1530,7 @@
     </row>
     <row r="2" spans="1:19" ht="17">
       <c r="A2" s="3" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1542,10 +1541,10 @@
       <c r="K2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="22" t="s">
+      <c r="L2" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="23"/>
+      <c r="M2" s="22"/>
     </row>
     <row r="3" spans="1:19" ht="17">
       <c r="A3" s="3" t="s">
@@ -1560,14 +1559,14 @@
       <c r="K3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="24" t="s">
+      <c r="L3" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="24"/>
+      <c r="M3" s="23"/>
     </row>
     <row r="4" spans="1:19" ht="17">
       <c r="A4" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1578,10 +1577,10 @@
       <c r="K4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="24" t="s">
+      <c r="L4" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="24"/>
+      <c r="M4" s="23"/>
     </row>
     <row r="5" spans="1:19" ht="17">
       <c r="A5" s="1"/>
@@ -1594,10 +1593,10 @@
       <c r="K5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="L5" s="24" t="s">
+      <c r="L5" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="24"/>
+      <c r="M5" s="23"/>
     </row>
     <row r="6" spans="1:19" ht="17">
       <c r="A6" s="1" t="s">
@@ -1612,41 +1611,41 @@
       <c r="K6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="L6" s="25" t="s">
+      <c r="L6" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="26"/>
+      <c r="M6" s="25"/>
     </row>
     <row r="7" spans="1:19" ht="17">
       <c r="A7" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:19">
-      <c r="I8" s="21" t="s">
+      <c r="I8" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="21"/>
-      <c r="O8" s="21"/>
-      <c r="P8" s="21"/>
-      <c r="Q8" s="19"/>
-      <c r="R8" s="19"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="18"/>
+      <c r="R8" s="18"/>
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>39</v>
@@ -1688,10 +1687,10 @@
         <v>24</v>
       </c>
       <c r="Q9" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="R9" s="4" t="s">
         <v>54</v>
-      </c>
-      <c r="R9" s="4" t="s">
-        <v>55</v>
       </c>
       <c r="S9" s="15" t="s">
         <v>40</v>
@@ -1717,7 +1716,7 @@
         <v>41647.986111111109</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I10" s="16">
         <v>41648.638888888891</v>
@@ -1740,10 +1739,10 @@
       <c r="O10" s="16">
         <v>41648.781944444447</v>
       </c>
-      <c r="Q10" s="20">
+      <c r="Q10" s="19">
         <v>-64.865799999999993</v>
       </c>
-      <c r="R10" s="20">
+      <c r="R10" s="19">
         <v>-64.260800000000003</v>
       </c>
     </row>
@@ -1767,7 +1766,7 @@
         <v>41647.986111111109</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I11" s="16">
         <v>41648.638888888891</v>
@@ -1790,10 +1789,10 @@
       <c r="O11" s="16">
         <v>41648.781944444447</v>
       </c>
-      <c r="Q11" s="20">
+      <c r="Q11" s="19">
         <v>-64.865799999999993</v>
       </c>
-      <c r="R11" s="20">
+      <c r="R11" s="19">
         <v>-64.260800000000003</v>
       </c>
     </row>
@@ -1817,7 +1816,7 @@
         <v>41647.986111111109</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I12" s="16">
         <v>41648.638888888891</v>
@@ -1840,10 +1839,10 @@
       <c r="O12" s="16">
         <v>41648.781944444447</v>
       </c>
-      <c r="Q12" s="20">
+      <c r="Q12" s="19">
         <v>-64.865799999999993</v>
       </c>
-      <c r="R12" s="20">
+      <c r="R12" s="19">
         <v>-64.260800000000003</v>
       </c>
     </row>
@@ -1867,7 +1866,7 @@
         <v>41647.986111111109</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I13" s="16">
         <v>41648.638888888891</v>
@@ -1890,10 +1889,10 @@
       <c r="O13" s="16">
         <v>41648.781944444447</v>
       </c>
-      <c r="Q13" s="20">
+      <c r="Q13" s="19">
         <v>-64.865799999999993</v>
       </c>
-      <c r="R13" s="20">
+      <c r="R13" s="19">
         <v>-64.260800000000003</v>
       </c>
     </row>
@@ -1917,7 +1916,7 @@
         <v>41647.986111111109</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I14" s="16">
         <v>41648.638888888891</v>
@@ -1940,10 +1939,10 @@
       <c r="O14" s="16">
         <v>41648.781944444447</v>
       </c>
-      <c r="Q14" s="20">
+      <c r="Q14" s="19">
         <v>-64.865799999999993</v>
       </c>
-      <c r="R14" s="20">
+      <c r="R14" s="19">
         <v>-64.260800000000003</v>
       </c>
     </row>
@@ -1967,7 +1966,7 @@
         <v>41647.986111111109</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I15" s="16">
         <v>41648.638888888891</v>
@@ -1990,10 +1989,10 @@
       <c r="O15" s="16">
         <v>41648.781944444447</v>
       </c>
-      <c r="Q15" s="20">
+      <c r="Q15" s="19">
         <v>-64.865799999999993</v>
       </c>
-      <c r="R15" s="20">
+      <c r="R15" s="19">
         <v>-64.260800000000003</v>
       </c>
     </row>
@@ -2017,7 +2016,7 @@
         <v>41647.986111111109</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I16" s="16">
         <v>41648.638888888891</v>
@@ -2040,10 +2039,10 @@
       <c r="O16" s="16">
         <v>41648.781944444447</v>
       </c>
-      <c r="Q16" s="20">
+      <c r="Q16" s="19">
         <v>-64.865799999999993</v>
       </c>
-      <c r="R16" s="20">
+      <c r="R16" s="19">
         <v>-64.260800000000003</v>
       </c>
     </row>
@@ -2067,7 +2066,7 @@
         <v>41647.986111111109</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I17" s="16">
         <v>41648.638888888891</v>
@@ -2090,10 +2089,10 @@
       <c r="O17" s="16">
         <v>41648.781944444447</v>
       </c>
-      <c r="Q17" s="20">
+      <c r="Q17" s="19">
         <v>-64.865799999999993</v>
       </c>
-      <c r="R17" s="20">
+      <c r="R17" s="19">
         <v>-64.260800000000003</v>
       </c>
     </row>
@@ -2117,7 +2116,7 @@
         <v>41648.927083333336</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I18" s="16">
         <v>41648.638888888891</v>
@@ -2143,10 +2142,10 @@
       <c r="P18" s="16">
         <v>41649.842361111114</v>
       </c>
-      <c r="Q18" s="20">
+      <c r="Q18" s="19">
         <v>-63.900599999999997</v>
       </c>
-      <c r="R18" s="20">
+      <c r="R18" s="19">
         <v>-66.715900000000005</v>
       </c>
     </row>
@@ -2170,7 +2169,7 @@
         <v>41648.927083333336</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I19" s="16">
         <v>41648.638888888891</v>
@@ -2196,10 +2195,10 @@
       <c r="P19" s="16">
         <v>41649.842361111114</v>
       </c>
-      <c r="Q19" s="20">
+      <c r="Q19" s="19">
         <v>-63.900599999999997</v>
       </c>
-      <c r="R19" s="20">
+      <c r="R19" s="19">
         <v>-66.715900000000005</v>
       </c>
     </row>
@@ -2223,7 +2222,7 @@
         <v>41648.927083333336</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I20" s="16">
         <v>41648.638888888891</v>
@@ -2249,10 +2248,10 @@
       <c r="P20" s="16">
         <v>41649.842361111114</v>
       </c>
-      <c r="Q20" s="20">
+      <c r="Q20" s="19">
         <v>-63.900599999999997</v>
       </c>
-      <c r="R20" s="20">
+      <c r="R20" s="19">
         <v>-66.715900000000005</v>
       </c>
     </row>
@@ -2276,7 +2275,7 @@
         <v>41648.927083333336</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I21" s="16">
         <v>41648.638888888891</v>
@@ -2302,10 +2301,10 @@
       <c r="P21" s="16">
         <v>41649.842361111114</v>
       </c>
-      <c r="Q21" s="20">
+      <c r="Q21" s="19">
         <v>-63.900599999999997</v>
       </c>
-      <c r="R21" s="20">
+      <c r="R21" s="19">
         <v>-66.715900000000005</v>
       </c>
     </row>
@@ -2329,7 +2328,7 @@
         <v>41648.927083333336</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I22" s="16">
         <v>41648.638888888891</v>
@@ -2355,10 +2354,10 @@
       <c r="P22" s="16">
         <v>41649.842361111114</v>
       </c>
-      <c r="Q22" s="20">
+      <c r="Q22" s="19">
         <v>-63.900599999999997</v>
       </c>
-      <c r="R22" s="20">
+      <c r="R22" s="19">
         <v>-66.715900000000005</v>
       </c>
     </row>
@@ -2382,7 +2381,7 @@
         <v>41648.927083333336</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I23" s="16">
         <v>41648.638888888891</v>
@@ -2408,10 +2407,10 @@
       <c r="P23" s="16">
         <v>41649.842361111114</v>
       </c>
-      <c r="Q23" s="20">
+      <c r="Q23" s="19">
         <v>-63.900599999999997</v>
       </c>
-      <c r="R23" s="20">
+      <c r="R23" s="19">
         <v>-66.715900000000005</v>
       </c>
     </row>
@@ -2435,7 +2434,7 @@
         <v>41648.927083333336</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I24" s="16">
         <v>41648.638888888891</v>
@@ -2461,10 +2460,10 @@
       <c r="P24" s="16">
         <v>41649.842361111114</v>
       </c>
-      <c r="Q24" s="20">
+      <c r="Q24" s="19">
         <v>-63.900599999999997</v>
       </c>
-      <c r="R24" s="20">
+      <c r="R24" s="19">
         <v>-66.715900000000005</v>
       </c>
     </row>
@@ -2488,7 +2487,7 @@
         <v>41649.729166666664</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I25" s="16">
         <v>41648.638888888891</v>
@@ -2511,10 +2510,10 @@
       <c r="P25" s="16">
         <v>41650.978472222225</v>
       </c>
-      <c r="Q25" s="20">
+      <c r="Q25" s="19">
         <v>-65.233800000000002</v>
       </c>
-      <c r="R25" s="20">
+      <c r="R25" s="19">
         <v>-66.775999999999996</v>
       </c>
     </row>
@@ -2538,7 +2537,7 @@
         <v>41649.729166666664</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I26" s="16">
         <v>41650.053472222222</v>
@@ -2561,10 +2560,10 @@
       <c r="P26" s="16">
         <v>41650.978472222225</v>
       </c>
-      <c r="Q26" s="20">
+      <c r="Q26" s="19">
         <v>-65.233800000000002</v>
       </c>
-      <c r="R26" s="20">
+      <c r="R26" s="19">
         <v>-66.775999999999996</v>
       </c>
     </row>
@@ -2588,7 +2587,7 @@
         <v>41649.729166666664</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I27" s="16">
         <v>41650.053472222222</v>
@@ -2611,10 +2610,10 @@
       <c r="P27" s="16">
         <v>41650.978472222225</v>
       </c>
-      <c r="Q27" s="20">
+      <c r="Q27" s="19">
         <v>-65.233800000000002</v>
       </c>
-      <c r="R27" s="20">
+      <c r="R27" s="19">
         <v>-66.775999999999996</v>
       </c>
     </row>
@@ -2638,7 +2637,7 @@
         <v>41649.729166666664</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I28" s="16">
         <v>41650.053472222222</v>
@@ -2661,10 +2660,10 @@
       <c r="P28" s="16">
         <v>41650.978472222225</v>
       </c>
-      <c r="Q28" s="20">
+      <c r="Q28" s="19">
         <v>-65.233800000000002</v>
       </c>
-      <c r="R28" s="20">
+      <c r="R28" s="19">
         <v>-66.775999999999996</v>
       </c>
     </row>
@@ -2688,7 +2687,7 @@
         <v>41649.729166666664</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I29" s="16">
         <v>41650.053472222222</v>
@@ -2711,10 +2710,10 @@
       <c r="P29" s="16">
         <v>41650.978472222225</v>
       </c>
-      <c r="Q29" s="20">
+      <c r="Q29" s="19">
         <v>-65.233800000000002</v>
       </c>
-      <c r="R29" s="20">
+      <c r="R29" s="19">
         <v>-66.775999999999996</v>
       </c>
     </row>
@@ -2738,7 +2737,7 @@
         <v>41649.729166666664</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I30" s="16">
         <v>41650.053472222222</v>
@@ -2761,10 +2760,10 @@
       <c r="P30" s="16">
         <v>41650.978472222225</v>
       </c>
-      <c r="Q30" s="20">
+      <c r="Q30" s="19">
         <v>-65.233800000000002</v>
       </c>
-      <c r="R30" s="20">
+      <c r="R30" s="19">
         <v>-66.775999999999996</v>
       </c>
     </row>
@@ -2788,7 +2787,7 @@
         <v>41649.729166666664</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I31" s="16">
         <v>41650.053472222222</v>
@@ -2811,1621 +2810,11 @@
       <c r="P31" s="16">
         <v>41650.978472222225</v>
       </c>
-      <c r="Q31" s="20">
+      <c r="Q31" s="19">
         <v>-65.233800000000002</v>
       </c>
-      <c r="R31" s="20">
+      <c r="R31" s="19">
         <v>-66.775999999999996</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18">
-      <c r="A32" s="2">
-        <v>18</v>
-      </c>
-      <c r="B32" s="2">
-        <v>300</v>
-      </c>
-      <c r="C32" s="17">
-        <v>0.1</v>
-      </c>
-      <c r="D32" s="2">
-        <v>0</v>
-      </c>
-      <c r="F32" s="2">
-        <v>1</v>
-      </c>
-      <c r="G32" s="16">
-        <v>41651.890277777777</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I32" s="16">
-        <v>41652.072916666664</v>
-      </c>
-      <c r="J32" s="16">
-        <v>41651.979166666664</v>
-      </c>
-      <c r="K32" s="16">
-        <v>41652.067361111112</v>
-      </c>
-      <c r="L32" s="16">
-        <v>41652.106944444444</v>
-      </c>
-      <c r="M32" s="16">
-        <v>41652.335416666669</v>
-      </c>
-      <c r="N32" s="16">
-        <v>41652.458333333336</v>
-      </c>
-      <c r="O32" s="16">
-        <v>41652.642361111109</v>
-      </c>
-      <c r="P32" s="16">
-        <v>41652.923611111109</v>
-      </c>
-      <c r="Q32" s="20">
-        <v>-66.505099999999999</v>
-      </c>
-      <c r="R32" s="20">
-        <v>-69.866699999999994</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18">
-      <c r="A33" s="2">
-        <v>18</v>
-      </c>
-      <c r="B33" s="2">
-        <v>300</v>
-      </c>
-      <c r="C33" s="17">
-        <v>0.1</v>
-      </c>
-      <c r="D33" s="2">
-        <v>10</v>
-      </c>
-      <c r="F33" s="2">
-        <v>1</v>
-      </c>
-      <c r="G33" s="16">
-        <v>41651.890277777777</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="I33" s="16">
-        <v>41652.072916666664</v>
-      </c>
-      <c r="J33" s="16">
-        <v>41651.979166666664</v>
-      </c>
-      <c r="K33" s="16">
-        <v>41652.067361111112</v>
-      </c>
-      <c r="L33" s="16">
-        <v>41652.106944444444</v>
-      </c>
-      <c r="M33" s="16">
-        <v>41652.335416666669</v>
-      </c>
-      <c r="N33" s="16">
-        <v>41652.458333333336</v>
-      </c>
-      <c r="O33" s="16">
-        <v>41652.642361111109</v>
-      </c>
-      <c r="P33" s="16">
-        <v>41652.923611111109</v>
-      </c>
-      <c r="Q33" s="20">
-        <v>-66.505099999999999</v>
-      </c>
-      <c r="R33" s="20">
-        <v>-69.866699999999994</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18">
-      <c r="A34" s="2">
-        <v>18</v>
-      </c>
-      <c r="B34" s="2">
-        <v>300</v>
-      </c>
-      <c r="C34" s="17">
-        <v>0.1</v>
-      </c>
-      <c r="D34" s="2">
-        <v>20</v>
-      </c>
-      <c r="F34" s="2">
-        <v>1</v>
-      </c>
-      <c r="G34" s="16">
-        <v>41651.890277777777</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="I34" s="16">
-        <v>41652.072916666664</v>
-      </c>
-      <c r="J34" s="16">
-        <v>41651.979166666664</v>
-      </c>
-      <c r="K34" s="16">
-        <v>41652.067361111112</v>
-      </c>
-      <c r="L34" s="16">
-        <v>41652.106944444444</v>
-      </c>
-      <c r="M34" s="16">
-        <v>41652.335416666669</v>
-      </c>
-      <c r="N34" s="16">
-        <v>41652.458333333336</v>
-      </c>
-      <c r="O34" s="16">
-        <v>41652.642361111109</v>
-      </c>
-      <c r="P34" s="16">
-        <v>41652.923611111109</v>
-      </c>
-      <c r="Q34" s="20">
-        <v>-66.505099999999999</v>
-      </c>
-      <c r="R34" s="20">
-        <v>-69.866699999999994</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18">
-      <c r="A35" s="2">
-        <v>18</v>
-      </c>
-      <c r="B35" s="2">
-        <v>300</v>
-      </c>
-      <c r="C35" s="17">
-        <v>0.1</v>
-      </c>
-      <c r="D35" s="2">
-        <v>40</v>
-      </c>
-      <c r="F35" s="2">
-        <v>1</v>
-      </c>
-      <c r="G35" s="16">
-        <v>41651.890277777777</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="I35" s="16">
-        <v>41652.072916666664</v>
-      </c>
-      <c r="J35" s="16">
-        <v>41651.979166666664</v>
-      </c>
-      <c r="K35" s="16">
-        <v>41652.067361111112</v>
-      </c>
-      <c r="L35" s="16">
-        <v>41652.106944444444</v>
-      </c>
-      <c r="M35" s="16">
-        <v>41652.335416666669</v>
-      </c>
-      <c r="N35" s="16">
-        <v>41652.458333333336</v>
-      </c>
-      <c r="O35" s="16">
-        <v>41652.642361111109</v>
-      </c>
-      <c r="P35" s="16">
-        <v>41652.923611111109</v>
-      </c>
-      <c r="Q35" s="20">
-        <v>-66.505099999999999</v>
-      </c>
-      <c r="R35" s="20">
-        <v>-69.866699999999994</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18">
-      <c r="A36" s="2">
-        <v>18</v>
-      </c>
-      <c r="B36" s="2">
-        <v>300</v>
-      </c>
-      <c r="C36" s="17">
-        <v>0.1</v>
-      </c>
-      <c r="D36" s="2">
-        <v>75</v>
-      </c>
-      <c r="F36" s="2">
-        <v>1</v>
-      </c>
-      <c r="G36" s="16">
-        <v>41651.890277777777</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I36" s="16">
-        <v>41652.072916666664</v>
-      </c>
-      <c r="J36" s="16">
-        <v>41651.979166666664</v>
-      </c>
-      <c r="K36" s="16">
-        <v>41652.067361111112</v>
-      </c>
-      <c r="L36" s="16">
-        <v>41652.106944444444</v>
-      </c>
-      <c r="M36" s="16">
-        <v>41652.335416666669</v>
-      </c>
-      <c r="N36" s="16">
-        <v>41652.458333333336</v>
-      </c>
-      <c r="O36" s="16">
-        <v>41652.642361111109</v>
-      </c>
-      <c r="P36" s="16">
-        <v>41652.923611111109</v>
-      </c>
-      <c r="Q36" s="20">
-        <v>-66.505099999999999</v>
-      </c>
-      <c r="R36" s="20">
-        <v>-69.866699999999994</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18">
-      <c r="A37" s="2">
-        <v>18</v>
-      </c>
-      <c r="B37" s="2">
-        <v>300</v>
-      </c>
-      <c r="C37" s="17">
-        <v>0.1</v>
-      </c>
-      <c r="D37" s="2">
-        <v>100</v>
-      </c>
-      <c r="F37" s="2">
-        <v>1</v>
-      </c>
-      <c r="G37" s="16">
-        <v>41651.890277777777</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I37" s="16">
-        <v>41652.072916666664</v>
-      </c>
-      <c r="J37" s="16">
-        <v>41651.979166666664</v>
-      </c>
-      <c r="K37" s="16">
-        <v>41652.067361111112</v>
-      </c>
-      <c r="L37" s="16">
-        <v>41652.106944444444</v>
-      </c>
-      <c r="M37" s="16">
-        <v>41652.335416666669</v>
-      </c>
-      <c r="N37" s="16">
-        <v>41652.458333333336</v>
-      </c>
-      <c r="O37" s="16">
-        <v>41652.642361111109</v>
-      </c>
-      <c r="P37" s="16">
-        <v>41652.923611111109</v>
-      </c>
-      <c r="Q37" s="20">
-        <v>-66.505099999999999</v>
-      </c>
-      <c r="R37" s="20">
-        <v>-69.866699999999994</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18">
-      <c r="A38" s="2">
-        <v>18</v>
-      </c>
-      <c r="B38" s="2">
-        <v>300</v>
-      </c>
-      <c r="C38" s="17">
-        <v>0.1</v>
-      </c>
-      <c r="D38" s="2">
-        <v>150</v>
-      </c>
-      <c r="F38" s="2">
-        <v>1</v>
-      </c>
-      <c r="G38" s="16">
-        <v>41651.890277777777</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="I38" s="16">
-        <v>41652.072916666664</v>
-      </c>
-      <c r="J38" s="16">
-        <v>41651.979166666664</v>
-      </c>
-      <c r="K38" s="16">
-        <v>41652.067361111112</v>
-      </c>
-      <c r="L38" s="16">
-        <v>41652.106944444444</v>
-      </c>
-      <c r="M38" s="16">
-        <v>41652.335416666669</v>
-      </c>
-      <c r="N38" s="16">
-        <v>41652.458333333336</v>
-      </c>
-      <c r="O38" s="16">
-        <v>41652.642361111109</v>
-      </c>
-      <c r="P38" s="16">
-        <v>41652.923611111109</v>
-      </c>
-      <c r="Q38" s="20">
-        <v>-66.505099999999999</v>
-      </c>
-      <c r="R38" s="20">
-        <v>-69.866699999999994</v>
-      </c>
-    </row>
-    <row r="39" spans="1:18">
-      <c r="A39" s="2">
-        <v>20</v>
-      </c>
-      <c r="B39" s="2">
-        <v>200</v>
-      </c>
-      <c r="C39" s="17">
-        <v>0.04</v>
-      </c>
-      <c r="D39" s="2">
-        <v>0</v>
-      </c>
-      <c r="G39" s="16">
-        <v>41652.704861111109</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I39" s="16">
-        <v>41652.072916666664</v>
-      </c>
-      <c r="J39" s="16">
-        <v>41652.790972222225</v>
-      </c>
-      <c r="K39" s="16"/>
-      <c r="L39" s="16">
-        <v>41653.071527777778</v>
-      </c>
-      <c r="N39" s="16">
-        <v>41653.56527777778</v>
-      </c>
-      <c r="O39" s="16">
-        <v>41653.698611111111</v>
-      </c>
-      <c r="Q39" s="20">
-        <v>-67.511099999999999</v>
-      </c>
-      <c r="R39" s="20">
-        <v>-70.589600000000004</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18">
-      <c r="A40" s="2">
-        <v>20</v>
-      </c>
-      <c r="B40" s="2">
-        <v>200</v>
-      </c>
-      <c r="C40" s="17">
-        <v>0.04</v>
-      </c>
-      <c r="D40" s="2">
-        <v>10</v>
-      </c>
-      <c r="G40" s="16">
-        <v>41652.704861111109</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="I40" s="16">
-        <v>41652.072916666664</v>
-      </c>
-      <c r="J40" s="16">
-        <v>41652.790972222225</v>
-      </c>
-      <c r="K40" s="16"/>
-      <c r="L40" s="16">
-        <v>41653.071527777778</v>
-      </c>
-      <c r="N40" s="16">
-        <v>41653.56527777778</v>
-      </c>
-      <c r="O40" s="16">
-        <v>41653.698611111111</v>
-      </c>
-      <c r="Q40" s="20">
-        <v>-67.511099999999999</v>
-      </c>
-      <c r="R40" s="20">
-        <v>-70.589600000000004</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18">
-      <c r="A41" s="2">
-        <v>20</v>
-      </c>
-      <c r="B41" s="2">
-        <v>200</v>
-      </c>
-      <c r="C41" s="17">
-        <v>0.04</v>
-      </c>
-      <c r="D41" s="2">
-        <v>15</v>
-      </c>
-      <c r="G41" s="16">
-        <v>41652.704861111109</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="I41" s="16">
-        <v>41652.072916666664</v>
-      </c>
-      <c r="J41" s="16">
-        <v>41652.790972222225</v>
-      </c>
-      <c r="K41" s="16"/>
-      <c r="L41" s="16">
-        <v>41653.071527777778</v>
-      </c>
-      <c r="N41" s="16">
-        <v>41653.56527777778</v>
-      </c>
-      <c r="O41" s="16">
-        <v>41653.698611111111</v>
-      </c>
-      <c r="Q41" s="20">
-        <v>-67.511099999999999</v>
-      </c>
-      <c r="R41" s="20">
-        <v>-70.589600000000004</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18">
-      <c r="A42" s="2">
-        <v>20</v>
-      </c>
-      <c r="B42" s="2">
-        <v>200</v>
-      </c>
-      <c r="C42" s="17">
-        <v>0.04</v>
-      </c>
-      <c r="D42" s="2">
-        <v>25</v>
-      </c>
-      <c r="G42" s="16">
-        <v>41652.704861111109</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="I42" s="16">
-        <v>41652.072916666664</v>
-      </c>
-      <c r="J42" s="16">
-        <v>41652.790972222225</v>
-      </c>
-      <c r="K42" s="16"/>
-      <c r="L42" s="16">
-        <v>41653.071527777778</v>
-      </c>
-      <c r="N42" s="16">
-        <v>41653.56527777778</v>
-      </c>
-      <c r="O42" s="16">
-        <v>41653.698611111111</v>
-      </c>
-      <c r="Q42" s="20">
-        <v>-67.511099999999999</v>
-      </c>
-      <c r="R42" s="20">
-        <v>-70.589600000000004</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18">
-      <c r="A43" s="2">
-        <v>20</v>
-      </c>
-      <c r="B43" s="2">
-        <v>200</v>
-      </c>
-      <c r="C43" s="17">
-        <v>0.04</v>
-      </c>
-      <c r="D43" s="2">
-        <v>40</v>
-      </c>
-      <c r="G43" s="16">
-        <v>41652.704861111109</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I43" s="16">
-        <v>41652.072916666664</v>
-      </c>
-      <c r="J43" s="16">
-        <v>41652.790972222225</v>
-      </c>
-      <c r="K43" s="16"/>
-      <c r="L43" s="16">
-        <v>41653.071527777778</v>
-      </c>
-      <c r="N43" s="16">
-        <v>41653.56527777778</v>
-      </c>
-      <c r="O43" s="16">
-        <v>41653.698611111111</v>
-      </c>
-      <c r="Q43" s="20">
-        <v>-67.511099999999999</v>
-      </c>
-      <c r="R43" s="20">
-        <v>-70.589600000000004</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18">
-      <c r="A44" s="2">
-        <v>20</v>
-      </c>
-      <c r="B44" s="2">
-        <v>200</v>
-      </c>
-      <c r="C44" s="17">
-        <v>0.04</v>
-      </c>
-      <c r="D44" s="2">
-        <v>75</v>
-      </c>
-      <c r="G44" s="16">
-        <v>41652.704861111109</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I44" s="16">
-        <v>41652.072916666664</v>
-      </c>
-      <c r="J44" s="16">
-        <v>41652.790972222225</v>
-      </c>
-      <c r="K44" s="16"/>
-      <c r="L44" s="16">
-        <v>41653.071527777778</v>
-      </c>
-      <c r="N44" s="16">
-        <v>41653.56527777778</v>
-      </c>
-      <c r="O44" s="16">
-        <v>41653.698611111111</v>
-      </c>
-      <c r="Q44" s="20">
-        <v>-67.511099999999999</v>
-      </c>
-      <c r="R44" s="20">
-        <v>-70.589600000000004</v>
-      </c>
-    </row>
-    <row r="45" spans="1:18">
-      <c r="A45" s="2">
-        <v>20</v>
-      </c>
-      <c r="B45" s="2">
-        <v>200</v>
-      </c>
-      <c r="C45" s="17">
-        <v>0.04</v>
-      </c>
-      <c r="D45" s="2">
-        <v>100</v>
-      </c>
-      <c r="G45" s="16">
-        <v>41652.704861111109</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="I45" s="16">
-        <v>41652.072916666664</v>
-      </c>
-      <c r="J45" s="16">
-        <v>41652.790972222225</v>
-      </c>
-      <c r="K45" s="16"/>
-      <c r="L45" s="16">
-        <v>41653.071527777778</v>
-      </c>
-      <c r="N45" s="16">
-        <v>41653.56527777778</v>
-      </c>
-      <c r="O45" s="16">
-        <v>41653.698611111111</v>
-      </c>
-      <c r="Q45" s="20">
-        <v>-67.511099999999999</v>
-      </c>
-      <c r="R45" s="20">
-        <v>-70.589600000000004</v>
-      </c>
-    </row>
-    <row r="46" spans="1:18">
-      <c r="A46" s="2">
-        <v>21</v>
-      </c>
-      <c r="B46" s="2">
-        <v>200</v>
-      </c>
-      <c r="C46" s="17">
-        <v>0</v>
-      </c>
-      <c r="D46" s="2">
-        <v>0</v>
-      </c>
-      <c r="F46" s="2">
-        <v>3.7</v>
-      </c>
-      <c r="G46" s="16">
-        <v>41653.628472222219</v>
-      </c>
-      <c r="H46" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I46" s="16">
-        <v>41653.67291666667</v>
-      </c>
-      <c r="J46" s="16">
-        <v>41653.65</v>
-      </c>
-      <c r="K46" s="16">
-        <v>41653.701388888891</v>
-      </c>
-      <c r="L46" s="16">
-        <v>41653.763194444444</v>
-      </c>
-      <c r="M46" s="16">
-        <v>41653.875694444447</v>
-      </c>
-      <c r="N46" s="16">
-        <v>41654.083333333336</v>
-      </c>
-      <c r="Q46" s="20">
-        <v>-67.772000000000006</v>
-      </c>
-      <c r="R46" s="20">
-        <v>-69.944500000000005</v>
-      </c>
-    </row>
-    <row r="47" spans="1:18">
-      <c r="A47" s="2">
-        <v>21</v>
-      </c>
-      <c r="B47" s="2">
-        <v>200</v>
-      </c>
-      <c r="C47" s="17">
-        <v>0</v>
-      </c>
-      <c r="D47" s="2">
-        <v>15</v>
-      </c>
-      <c r="F47" s="2">
-        <v>3.7</v>
-      </c>
-      <c r="G47" s="16">
-        <v>41653.628472222219</v>
-      </c>
-      <c r="H47" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="I47" s="16">
-        <v>41653.67291666667</v>
-      </c>
-      <c r="J47" s="16">
-        <v>41653.65</v>
-      </c>
-      <c r="K47" s="16">
-        <v>41653.701388888891</v>
-      </c>
-      <c r="L47" s="18">
-        <v>41653.763194444444</v>
-      </c>
-      <c r="M47" s="16">
-        <v>41653.875694444447</v>
-      </c>
-      <c r="N47" s="16">
-        <v>41654.083333333336</v>
-      </c>
-      <c r="Q47" s="20">
-        <v>-67.772000000000006</v>
-      </c>
-      <c r="R47" s="20">
-        <v>-69.944500000000005</v>
-      </c>
-    </row>
-    <row r="48" spans="1:18">
-      <c r="A48" s="2">
-        <v>21</v>
-      </c>
-      <c r="B48" s="2">
-        <v>200</v>
-      </c>
-      <c r="C48" s="17">
-        <v>0</v>
-      </c>
-      <c r="D48" s="2">
-        <v>30</v>
-      </c>
-      <c r="F48" s="2">
-        <v>3.7</v>
-      </c>
-      <c r="G48" s="16">
-        <v>41653.628472222219</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="I48" s="16">
-        <v>41653.67291666667</v>
-      </c>
-      <c r="J48" s="16">
-        <v>41653.65</v>
-      </c>
-      <c r="K48" s="16">
-        <v>41653.701388888891</v>
-      </c>
-      <c r="L48" s="18">
-        <v>41653.763194444444</v>
-      </c>
-      <c r="M48" s="16">
-        <v>41653.875694444447</v>
-      </c>
-      <c r="N48" s="16">
-        <v>41654.083333333336</v>
-      </c>
-      <c r="Q48" s="20">
-        <v>-67.772000000000006</v>
-      </c>
-      <c r="R48" s="20">
-        <v>-69.944500000000005</v>
-      </c>
-    </row>
-    <row r="49" spans="1:18">
-      <c r="A49" s="2">
-        <v>21</v>
-      </c>
-      <c r="B49" s="2">
-        <v>200</v>
-      </c>
-      <c r="C49" s="17">
-        <v>0</v>
-      </c>
-      <c r="D49" s="2">
-        <v>50</v>
-      </c>
-      <c r="F49" s="2">
-        <v>3.7</v>
-      </c>
-      <c r="G49" s="16">
-        <v>41653.628472222219</v>
-      </c>
-      <c r="H49" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="I49" s="16">
-        <v>41653.67291666667</v>
-      </c>
-      <c r="J49" s="16">
-        <v>41653.65</v>
-      </c>
-      <c r="K49" s="16">
-        <v>41653.701388888891</v>
-      </c>
-      <c r="L49" s="18">
-        <v>41653.763194444444</v>
-      </c>
-      <c r="M49" s="16">
-        <v>41653.875694444447</v>
-      </c>
-      <c r="N49" s="16">
-        <v>41654.083333333336</v>
-      </c>
-      <c r="Q49" s="20">
-        <v>-67.772000000000006</v>
-      </c>
-      <c r="R49" s="20">
-        <v>-69.944500000000005</v>
-      </c>
-    </row>
-    <row r="50" spans="1:18">
-      <c r="A50" s="2">
-        <v>21</v>
-      </c>
-      <c r="B50" s="2">
-        <v>200</v>
-      </c>
-      <c r="C50" s="17">
-        <v>0</v>
-      </c>
-      <c r="D50" s="2">
-        <v>80</v>
-      </c>
-      <c r="F50" s="2">
-        <v>3.7</v>
-      </c>
-      <c r="G50" s="16">
-        <v>41653.628472222219</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I50" s="16">
-        <v>41653.67291666667</v>
-      </c>
-      <c r="J50" s="16">
-        <v>41653.65</v>
-      </c>
-      <c r="K50" s="16">
-        <v>41653.701388888891</v>
-      </c>
-      <c r="L50" s="18">
-        <v>41653.763194444444</v>
-      </c>
-      <c r="M50" s="16">
-        <v>41653.875694444447</v>
-      </c>
-      <c r="N50" s="16">
-        <v>41654.083333333336</v>
-      </c>
-      <c r="Q50" s="20">
-        <v>-67.772000000000006</v>
-      </c>
-      <c r="R50" s="20">
-        <v>-69.944500000000005</v>
-      </c>
-    </row>
-    <row r="51" spans="1:18">
-      <c r="A51" s="2">
-        <v>21</v>
-      </c>
-      <c r="B51" s="2">
-        <v>200</v>
-      </c>
-      <c r="C51" s="17">
-        <v>0</v>
-      </c>
-      <c r="D51" s="2">
-        <v>100</v>
-      </c>
-      <c r="F51" s="2">
-        <v>3.7</v>
-      </c>
-      <c r="G51" s="16">
-        <v>41653.628472222219</v>
-      </c>
-      <c r="H51" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I51" s="16">
-        <v>41653.67291666667</v>
-      </c>
-      <c r="J51" s="16">
-        <v>41653.65</v>
-      </c>
-      <c r="K51" s="16">
-        <v>41653.701388888891</v>
-      </c>
-      <c r="L51" s="18">
-        <v>41653.763194444444</v>
-      </c>
-      <c r="M51" s="16">
-        <v>41653.875694444447</v>
-      </c>
-      <c r="N51" s="16">
-        <v>41654.083333333336</v>
-      </c>
-      <c r="Q51" s="20">
-        <v>-67.772000000000006</v>
-      </c>
-      <c r="R51" s="20">
-        <v>-69.944500000000005</v>
-      </c>
-    </row>
-    <row r="52" spans="1:18">
-      <c r="A52" s="2">
-        <v>21</v>
-      </c>
-      <c r="B52" s="2">
-        <v>200</v>
-      </c>
-      <c r="C52" s="17">
-        <v>0</v>
-      </c>
-      <c r="D52" s="2">
-        <v>150</v>
-      </c>
-      <c r="F52" s="2">
-        <v>3.7</v>
-      </c>
-      <c r="G52" s="16">
-        <v>41653.628472222219</v>
-      </c>
-      <c r="H52" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="I52" s="16">
-        <v>41653.67291666667</v>
-      </c>
-      <c r="J52" s="16">
-        <v>41653.65</v>
-      </c>
-      <c r="K52" s="16">
-        <v>41653.701388888891</v>
-      </c>
-      <c r="L52" s="18">
-        <v>41653.763194444444</v>
-      </c>
-      <c r="M52" s="16">
-        <v>41653.875694444447</v>
-      </c>
-      <c r="N52" s="16">
-        <v>41654.083333333336</v>
-      </c>
-      <c r="Q52" s="20">
-        <v>-67.772000000000006</v>
-      </c>
-      <c r="R52" s="20">
-        <v>-69.944500000000005</v>
-      </c>
-    </row>
-    <row r="53" spans="1:18">
-      <c r="A53" s="2">
-        <v>30</v>
-      </c>
-      <c r="B53" s="2">
-        <v>200</v>
-      </c>
-      <c r="C53" s="17">
-        <v>-0.08</v>
-      </c>
-      <c r="D53" s="2">
-        <v>0</v>
-      </c>
-      <c r="G53" s="16">
-        <v>41656.8125</v>
-      </c>
-      <c r="H53" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I53" s="16">
-        <v>41656.877083333333</v>
-      </c>
-      <c r="J53" s="16">
-        <v>41656.85833333333</v>
-      </c>
-      <c r="K53" s="16">
-        <v>41656.915277777778</v>
-      </c>
-      <c r="L53" s="16">
-        <v>41656.961111111108</v>
-      </c>
-      <c r="Q53" s="20">
-        <v>-68.286199999999994</v>
-      </c>
-      <c r="R53" s="20">
-        <v>-68.610299999999995</v>
-      </c>
-    </row>
-    <row r="54" spans="1:18">
-      <c r="A54" s="2">
-        <v>30</v>
-      </c>
-      <c r="B54" s="2">
-        <v>200</v>
-      </c>
-      <c r="C54" s="17">
-        <v>-0.08</v>
-      </c>
-      <c r="D54" s="2">
-        <v>5</v>
-      </c>
-      <c r="G54" s="16">
-        <v>41656.8125</v>
-      </c>
-      <c r="H54" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="I54" s="16">
-        <v>41656.877083333333</v>
-      </c>
-      <c r="J54" s="16">
-        <v>41656.85833333333</v>
-      </c>
-      <c r="K54" s="16">
-        <v>41656.915277777778</v>
-      </c>
-      <c r="L54" s="16">
-        <v>41656.961111111108</v>
-      </c>
-      <c r="Q54" s="20">
-        <v>-68.286199999999994</v>
-      </c>
-      <c r="R54" s="20">
-        <v>-68.610299999999995</v>
-      </c>
-    </row>
-    <row r="55" spans="1:18">
-      <c r="A55" s="2">
-        <v>30</v>
-      </c>
-      <c r="B55" s="2">
-        <v>200</v>
-      </c>
-      <c r="C55" s="17">
-        <v>-0.08</v>
-      </c>
-      <c r="D55" s="2">
-        <v>15</v>
-      </c>
-      <c r="G55" s="16">
-        <v>41656.8125</v>
-      </c>
-      <c r="H55" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="I55" s="16">
-        <v>41656.877083333333</v>
-      </c>
-      <c r="J55" s="16">
-        <v>41656.85833333333</v>
-      </c>
-      <c r="K55" s="16">
-        <v>41656.915277777778</v>
-      </c>
-      <c r="L55" s="16">
-        <v>41656.961111111108</v>
-      </c>
-      <c r="Q55" s="20">
-        <v>-68.286199999999994</v>
-      </c>
-      <c r="R55" s="20">
-        <v>-68.610299999999995</v>
-      </c>
-    </row>
-    <row r="56" spans="1:18">
-      <c r="A56" s="2">
-        <v>30</v>
-      </c>
-      <c r="B56" s="2">
-        <v>200</v>
-      </c>
-      <c r="C56" s="17">
-        <v>-0.08</v>
-      </c>
-      <c r="D56" s="2">
-        <v>30</v>
-      </c>
-      <c r="G56" s="16">
-        <v>41656.8125</v>
-      </c>
-      <c r="H56" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="I56" s="16">
-        <v>41656.877083333333</v>
-      </c>
-      <c r="J56" s="16">
-        <v>41656.85833333333</v>
-      </c>
-      <c r="K56" s="16">
-        <v>41656.915277777778</v>
-      </c>
-      <c r="L56" s="16">
-        <v>41656.961111111108</v>
-      </c>
-      <c r="Q56" s="20">
-        <v>-68.286199999999994</v>
-      </c>
-      <c r="R56" s="20">
-        <v>-68.610299999999995</v>
-      </c>
-    </row>
-    <row r="57" spans="1:18">
-      <c r="A57" s="2">
-        <v>30</v>
-      </c>
-      <c r="B57" s="2">
-        <v>200</v>
-      </c>
-      <c r="C57" s="17">
-        <v>-0.08</v>
-      </c>
-      <c r="D57" s="2">
-        <v>50</v>
-      </c>
-      <c r="G57" s="16">
-        <v>41656.8125</v>
-      </c>
-      <c r="H57" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I57" s="16">
-        <v>41656.877083333333</v>
-      </c>
-      <c r="J57" s="16">
-        <v>41656.85833333333</v>
-      </c>
-      <c r="K57" s="16">
-        <v>41656.915277777778</v>
-      </c>
-      <c r="L57" s="16">
-        <v>41656.961111111108</v>
-      </c>
-      <c r="Q57" s="20">
-        <v>-68.286199999999994</v>
-      </c>
-      <c r="R57" s="20">
-        <v>-68.610299999999995</v>
-      </c>
-    </row>
-    <row r="58" spans="1:18">
-      <c r="A58" s="2">
-        <v>30</v>
-      </c>
-      <c r="B58" s="2">
-        <v>200</v>
-      </c>
-      <c r="C58" s="17">
-        <v>-0.08</v>
-      </c>
-      <c r="D58" s="2">
-        <v>75</v>
-      </c>
-      <c r="G58" s="16">
-        <v>41656.8125</v>
-      </c>
-      <c r="H58" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I58" s="16">
-        <v>41656.877083333333</v>
-      </c>
-      <c r="J58" s="16">
-        <v>41656.85833333333</v>
-      </c>
-      <c r="K58" s="16">
-        <v>41656.915277777778</v>
-      </c>
-      <c r="L58" s="16">
-        <v>41656.961111111108</v>
-      </c>
-      <c r="Q58" s="20">
-        <v>-68.286199999999994</v>
-      </c>
-      <c r="R58" s="20">
-        <v>-68.610299999999995</v>
-      </c>
-    </row>
-    <row r="59" spans="1:18">
-      <c r="A59" s="2">
-        <v>30</v>
-      </c>
-      <c r="B59" s="2">
-        <v>200</v>
-      </c>
-      <c r="C59" s="17">
-        <v>-0.08</v>
-      </c>
-      <c r="D59" s="2">
-        <v>100</v>
-      </c>
-      <c r="G59" s="16">
-        <v>41656.8125</v>
-      </c>
-      <c r="H59" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="I59" s="16">
-        <v>41656.877083333333</v>
-      </c>
-      <c r="J59" s="16">
-        <v>41656.85833333333</v>
-      </c>
-      <c r="K59" s="16">
-        <v>41656.915277777778</v>
-      </c>
-      <c r="L59" s="16">
-        <v>41656.961111111108</v>
-      </c>
-      <c r="Q59" s="20">
-        <v>-68.286199999999994</v>
-      </c>
-      <c r="R59" s="20">
-        <v>-68.610299999999995</v>
-      </c>
-    </row>
-    <row r="60" spans="1:18">
-      <c r="A60" s="2">
-        <v>47</v>
-      </c>
-      <c r="B60" s="2">
-        <v>500</v>
-      </c>
-      <c r="C60" s="17">
-        <v>0.06</v>
-      </c>
-      <c r="D60" s="2">
-        <v>0</v>
-      </c>
-      <c r="G60" s="16">
-        <v>41662.697916666664</v>
-      </c>
-      <c r="H60" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="I60" s="16">
-        <v>41662.794444444444</v>
-      </c>
-      <c r="J60" s="16">
-        <v>41662.772916666669</v>
-      </c>
-      <c r="K60" s="16">
-        <v>41662.818749999999</v>
-      </c>
-      <c r="L60" s="16">
-        <v>41662.878472222219</v>
-      </c>
-      <c r="M60" s="16">
-        <v>41663.037499999999</v>
-      </c>
-      <c r="N60" s="16">
-        <v>41663.380555555559</v>
-      </c>
-      <c r="O60" s="16">
-        <v>41663.522222222222</v>
-      </c>
-      <c r="P60" s="16">
-        <v>41663.79791666667</v>
-      </c>
-      <c r="Q60" s="2">
-        <v>-65.48</v>
-      </c>
-      <c r="R60" s="2">
-        <v>-66.150000000000006</v>
-      </c>
-    </row>
-    <row r="61" spans="1:18">
-      <c r="A61" s="2">
-        <v>47</v>
-      </c>
-      <c r="B61" s="2">
-        <v>500</v>
-      </c>
-      <c r="C61" s="17">
-        <v>0.06</v>
-      </c>
-      <c r="D61" s="2">
-        <v>10</v>
-      </c>
-      <c r="G61" s="16">
-        <v>41662.697916666664</v>
-      </c>
-      <c r="H61" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="I61" s="16">
-        <v>41662.794444444444</v>
-      </c>
-      <c r="J61" s="16">
-        <v>41662.772916666669</v>
-      </c>
-      <c r="K61" s="16">
-        <v>41662.818749999999</v>
-      </c>
-      <c r="L61" s="16">
-        <v>41662.878472222219</v>
-      </c>
-      <c r="M61" s="16">
-        <v>41663.037499999999</v>
-      </c>
-      <c r="N61" s="16">
-        <v>41663.380555555559</v>
-      </c>
-      <c r="O61" s="16">
-        <v>41663.522222222222</v>
-      </c>
-      <c r="P61" s="16">
-        <v>41663.79791666667</v>
-      </c>
-      <c r="Q61" s="2">
-        <v>-65.48</v>
-      </c>
-      <c r="R61" s="2">
-        <v>-66.150000000000006</v>
-      </c>
-    </row>
-    <row r="62" spans="1:18">
-      <c r="A62" s="2">
-        <v>47</v>
-      </c>
-      <c r="B62" s="2">
-        <v>500</v>
-      </c>
-      <c r="C62" s="17">
-        <v>0.06</v>
-      </c>
-      <c r="D62" s="2">
-        <v>20</v>
-      </c>
-      <c r="G62" s="16">
-        <v>41662.697916666664</v>
-      </c>
-      <c r="H62" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="I62" s="16">
-        <v>41662.794444444444</v>
-      </c>
-      <c r="J62" s="16">
-        <v>41662.772916666669</v>
-      </c>
-      <c r="K62" s="16">
-        <v>41662.818749999999</v>
-      </c>
-      <c r="L62" s="16">
-        <v>41662.878472222219</v>
-      </c>
-      <c r="M62" s="16">
-        <v>41663.037499999999</v>
-      </c>
-      <c r="N62" s="16">
-        <v>41663.380555555559</v>
-      </c>
-      <c r="O62" s="16">
-        <v>41663.522222222222</v>
-      </c>
-      <c r="P62" s="16">
-        <v>41663.79791666667</v>
-      </c>
-      <c r="Q62" s="2">
-        <v>-65.48</v>
-      </c>
-      <c r="R62" s="2">
-        <v>-66.150000000000006</v>
-      </c>
-    </row>
-    <row r="63" spans="1:18">
-      <c r="A63" s="2">
-        <v>47</v>
-      </c>
-      <c r="B63" s="2">
-        <v>500</v>
-      </c>
-      <c r="C63" s="17">
-        <v>0.06</v>
-      </c>
-      <c r="D63" s="2">
-        <v>35</v>
-      </c>
-      <c r="G63" s="16">
-        <v>41662.697916666664</v>
-      </c>
-      <c r="H63" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="I63" s="16">
-        <v>41662.794444444444</v>
-      </c>
-      <c r="J63" s="16">
-        <v>41662.772916666669</v>
-      </c>
-      <c r="K63" s="16">
-        <v>41662.818749999999</v>
-      </c>
-      <c r="L63" s="16">
-        <v>41662.878472222219</v>
-      </c>
-      <c r="M63" s="16">
-        <v>41663.037499999999</v>
-      </c>
-      <c r="N63" s="16">
-        <v>41663.380555555559</v>
-      </c>
-      <c r="O63" s="16">
-        <v>41663.522222222222</v>
-      </c>
-      <c r="P63" s="16">
-        <v>41663.79791666667</v>
-      </c>
-      <c r="Q63" s="2">
-        <v>-65.48</v>
-      </c>
-      <c r="R63" s="2">
-        <v>-66.150000000000006</v>
-      </c>
-    </row>
-    <row r="64" spans="1:18">
-      <c r="A64" s="2">
-        <v>47</v>
-      </c>
-      <c r="B64" s="2">
-        <v>500</v>
-      </c>
-      <c r="C64" s="17">
-        <v>0.06</v>
-      </c>
-      <c r="D64" s="2">
-        <v>50</v>
-      </c>
-      <c r="G64" s="16">
-        <v>41662.697916666664</v>
-      </c>
-      <c r="H64" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I64" s="16">
-        <v>41662.794444444444</v>
-      </c>
-      <c r="J64" s="16">
-        <v>41662.772916666669</v>
-      </c>
-      <c r="K64" s="16">
-        <v>41662.818749999999</v>
-      </c>
-      <c r="L64" s="16">
-        <v>41662.878472222219</v>
-      </c>
-      <c r="M64" s="16">
-        <v>41663.037499999999</v>
-      </c>
-      <c r="N64" s="16">
-        <v>41663.380555555559</v>
-      </c>
-      <c r="O64" s="16">
-        <v>41663.522222222222</v>
-      </c>
-      <c r="P64" s="16">
-        <v>41663.79791666667</v>
-      </c>
-      <c r="Q64" s="2">
-        <v>-65.48</v>
-      </c>
-      <c r="R64" s="2">
-        <v>-66.150000000000006</v>
-      </c>
-    </row>
-    <row r="65" spans="1:18">
-      <c r="A65" s="2">
-        <v>47</v>
-      </c>
-      <c r="B65" s="2">
-        <v>500</v>
-      </c>
-      <c r="C65" s="17">
-        <v>0.06</v>
-      </c>
-      <c r="D65" s="2">
-        <v>70</v>
-      </c>
-      <c r="G65" s="16">
-        <v>41662.697916666664</v>
-      </c>
-      <c r="H65" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I65" s="16">
-        <v>41662.794444444444</v>
-      </c>
-      <c r="J65" s="16">
-        <v>41662.772916666669</v>
-      </c>
-      <c r="K65" s="16">
-        <v>41662.818749999999</v>
-      </c>
-      <c r="L65" s="16">
-        <v>41662.878472222219</v>
-      </c>
-      <c r="M65" s="16">
-        <v>41663.037499999999</v>
-      </c>
-      <c r="N65" s="16">
-        <v>41663.380555555559</v>
-      </c>
-      <c r="O65" s="16">
-        <v>41663.522222222222</v>
-      </c>
-      <c r="P65" s="16">
-        <v>41663.79791666667</v>
-      </c>
-      <c r="Q65" s="2">
-        <v>-65.48</v>
-      </c>
-      <c r="R65" s="2">
-        <v>-66.150000000000006</v>
-      </c>
-    </row>
-    <row r="66" spans="1:18">
-      <c r="A66" s="2">
-        <v>47</v>
-      </c>
-      <c r="B66" s="2">
-        <v>500</v>
-      </c>
-      <c r="C66" s="17">
-        <v>0.06</v>
-      </c>
-      <c r="D66" s="2">
-        <v>100</v>
-      </c>
-      <c r="G66" s="16">
-        <v>41662.697916666664</v>
-      </c>
-      <c r="H66" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="I66" s="16">
-        <v>41662.794444444444</v>
-      </c>
-      <c r="J66" s="16">
-        <v>41662.772916666669</v>
-      </c>
-      <c r="K66" s="16">
-        <v>41662.818749999999</v>
-      </c>
-      <c r="L66" s="16">
-        <v>41662.878472222219</v>
-      </c>
-      <c r="M66" s="16">
-        <v>41663.037499999999</v>
-      </c>
-      <c r="N66" s="16">
-        <v>41663.380555555559</v>
-      </c>
-      <c r="O66" s="16">
-        <v>41663.522222222222</v>
-      </c>
-      <c r="P66" s="16">
-        <v>41663.79791666667</v>
-      </c>
-      <c r="Q66" s="2">
-        <v>-65.48</v>
-      </c>
-      <c r="R66" s="2">
-        <v>-66.150000000000006</v>
       </c>
     </row>
   </sheetData>
@@ -4596,18 +2985,18 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1">
-      <c r="G8" s="27" t="s">
+      <c r="G8" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="27"/>
+      <c r="H8" s="26"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
     </row>
     <row r="11" spans="1:8">
       <c r="G11" s="9"/>
@@ -4859,16 +3248,16 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="36" customHeight="1">
-      <c r="A32" s="28" t="s">
+      <c r="A32" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="28"/>
-      <c r="C32" s="28"/>
-      <c r="D32" s="28"/>
-      <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="28"/>
-      <c r="H32" s="28"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="27"/>
+      <c r="E32" s="27"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="27"/>
+      <c r="H32" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>